<commit_message>
dia de semana fixo corrigido
</commit_message>
<xml_diff>
--- a/relatorios/relatorio_frequencia_141025.xlsx
+++ b/relatorios/relatorio_frequencia_141025.xlsx
@@ -503,7 +503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,7 +520,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Relatório de Frequência - Terça-feira, 14/10/2025</t>
+          <t>Relatório de Frequência - Terã§a-feira, 14/10/2025</t>
         </is>
       </c>
     </row>
@@ -604,89 +604,89 @@
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
+          <t>2025000711</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>Camile Victória Müller Beazussi</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
           <t>2024000400</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>Isabela Moreira Fernandes</t>
         </is>
       </c>
-      <c r="C7" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D7" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="8"/>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="9"/>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>TURMA: EF1602</t>
         </is>
       </c>
-      <c r="B9" s="3" t="n"/>
-      <c r="C9" s="3" t="n"/>
-      <c r="D9" s="4" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="inlineStr">
+      <c r="B10" s="3" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="4" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B10" s="5" t="inlineStr">
+      <c r="B11" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C10" s="5" t="inlineStr">
+      <c r="C11" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D10" s="5" t="inlineStr">
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>2025000687</t>
-        </is>
-      </c>
-      <c r="B11" s="6" t="inlineStr">
-        <is>
-          <t>Alice Velasco Rigobello</t>
-        </is>
-      </c>
-      <c r="C11" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D11" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>2024000527</t>
+          <t>2025000687</t>
         </is>
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>Isabela de Souza Tauil Paladino</t>
+          <t>Alice Velasco Rigobello</t>
         </is>
       </c>
       <c r="C12" s="6" t="inlineStr">
@@ -703,12 +703,12 @@
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
         <is>
-          <t>2022321427</t>
+          <t>2024000527</t>
         </is>
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
-          <t>Larissa Ferreira de Paula</t>
+          <t>Isabela de Souza Tauil Paladino</t>
         </is>
       </c>
       <c r="C13" s="6" t="inlineStr">
@@ -725,12 +725,12 @@
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
         <is>
-          <t>2023000255</t>
+          <t>2022321427</t>
         </is>
       </c>
       <c r="B14" s="6" t="inlineStr">
         <is>
-          <t>Laura Pereira da Silva</t>
+          <t>Larissa Ferreira de Paula</t>
         </is>
       </c>
       <c r="C14" s="6" t="inlineStr">
@@ -747,12 +747,12 @@
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
         <is>
-          <t>2561001116</t>
+          <t>2023000255</t>
         </is>
       </c>
       <c r="B15" s="6" t="inlineStr">
         <is>
-          <t>Manuela Soares Gentil</t>
+          <t>Laura Pereira da Silva</t>
         </is>
       </c>
       <c r="C15" s="6" t="inlineStr">
@@ -769,111 +769,111 @@
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
         <is>
+          <t>2561001116</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>Manuela Soares Gentil</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D16" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
           <t>2022321349</t>
         </is>
       </c>
-      <c r="B16" s="6" t="inlineStr">
+      <c r="B17" s="6" t="inlineStr">
         <is>
           <t>Maria Clara Lopes Chaves</t>
         </is>
       </c>
-      <c r="C16" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D16" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="7" t="inlineStr">
+      <c r="C17" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D17" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
         <is>
           <t>2025000685</t>
         </is>
       </c>
-      <c r="B17" s="7" t="inlineStr">
+      <c r="B18" s="7" t="inlineStr">
         <is>
           <t>Miguel Muniz Rodrigues</t>
         </is>
       </c>
-      <c r="C17" s="7" t="inlineStr">
+      <c r="C18" s="7" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D17" s="7" t="inlineStr">
+      <c r="D18" s="7" t="inlineStr">
         <is>
           <t>Saída: 10:46:45</t>
         </is>
       </c>
     </row>
-    <row r="18"/>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
+    <row r="19"/>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>TURMA: EF1701</t>
         </is>
       </c>
-      <c r="B19" s="3" t="n"/>
-      <c r="C19" s="3" t="n"/>
-      <c r="D19" s="4" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="inlineStr">
+      <c r="B20" s="3" t="n"/>
+      <c r="C20" s="3" t="n"/>
+      <c r="D20" s="4" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B20" s="5" t="inlineStr">
+      <c r="B21" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C20" s="5" t="inlineStr">
+      <c r="C21" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D20" s="5" t="inlineStr">
+      <c r="D21" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="inlineStr">
-        <is>
-          <t>2022321034</t>
-        </is>
-      </c>
-      <c r="B21" s="6" t="inlineStr">
-        <is>
-          <t>Alice Gaudard Hespanhol</t>
-        </is>
-      </c>
-      <c r="C21" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D21" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
         <is>
-          <t>2024000417</t>
+          <t>2022321034</t>
         </is>
       </c>
       <c r="B22" s="6" t="inlineStr">
         <is>
-          <t>Helena Ferreira Monteiro</t>
+          <t>Alice Gaudard Hespanhol</t>
         </is>
       </c>
       <c r="C22" s="6" t="inlineStr">
@@ -890,12 +890,12 @@
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
         <is>
-          <t>2025000693</t>
+          <t>2024000417</t>
         </is>
       </c>
       <c r="B23" s="6" t="inlineStr">
         <is>
-          <t>Marcella Santos Vasconcelos</t>
+          <t>Helena Ferreira Monteiro</t>
         </is>
       </c>
       <c r="C23" s="6" t="inlineStr">
@@ -912,12 +912,12 @@
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
         <is>
-          <t>2025000691</t>
+          <t>2025000693</t>
         </is>
       </c>
       <c r="B24" s="6" t="inlineStr">
         <is>
-          <t>Roberta França Corrêa</t>
+          <t>Marcella Santos Vasconcelos</t>
         </is>
       </c>
       <c r="C24" s="6" t="inlineStr">
@@ -934,111 +934,111 @@
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
         <is>
+          <t>2025000691</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>Roberta França Corrêa</t>
+        </is>
+      </c>
+      <c r="C25" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D25" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
           <t>2024000411</t>
         </is>
       </c>
-      <c r="B25" s="6" t="inlineStr">
+      <c r="B26" s="6" t="inlineStr">
         <is>
           <t>Sofia Riberto Batalha</t>
         </is>
       </c>
-      <c r="C25" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D25" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="7" t="inlineStr">
+      <c r="C26" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D26" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
         <is>
           <t>2022321377</t>
         </is>
       </c>
-      <c r="B26" s="7" t="inlineStr">
+      <c r="B27" s="7" t="inlineStr">
         <is>
           <t>Vítor Nogueira Gonçalves</t>
         </is>
       </c>
-      <c r="C26" s="7" t="inlineStr">
+      <c r="C27" s="7" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D26" s="7" t="inlineStr">
+      <c r="D27" s="7" t="inlineStr">
         <is>
           <t>Saída: 11:31:51</t>
         </is>
       </c>
     </row>
-    <row r="27"/>
-    <row r="28">
-      <c r="A28" s="2" t="inlineStr">
+    <row r="28"/>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
         <is>
           <t>TURMA: EF1702</t>
         </is>
       </c>
-      <c r="B28" s="3" t="n"/>
-      <c r="C28" s="3" t="n"/>
-      <c r="D28" s="4" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="5" t="inlineStr">
+      <c r="B29" s="3" t="n"/>
+      <c r="C29" s="3" t="n"/>
+      <c r="D29" s="4" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B29" s="5" t="inlineStr">
+      <c r="B30" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C29" s="5" t="inlineStr">
+      <c r="C30" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D29" s="5" t="inlineStr">
+      <c r="D30" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="6" t="inlineStr">
-        <is>
-          <t>2022321341</t>
-        </is>
-      </c>
-      <c r="B30" s="6" t="inlineStr">
-        <is>
-          <t>Arthur da Silva Pessoa</t>
-        </is>
-      </c>
-      <c r="C30" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D30" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
         <is>
-          <t>2022321470</t>
+          <t>2022321341</t>
         </is>
       </c>
       <c r="B31" s="6" t="inlineStr">
         <is>
-          <t>Maria Eduarda Rodrigues Pimentel</t>
+          <t>Arthur da Silva Pessoa</t>
         </is>
       </c>
       <c r="C31" s="6" t="inlineStr">
@@ -1055,430 +1055,430 @@
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
         <is>
+          <t>2022321470</t>
+        </is>
+      </c>
+      <c r="B32" s="6" t="inlineStr">
+        <is>
+          <t>Maria Eduarda Rodrigues Pimentel</t>
+        </is>
+      </c>
+      <c r="C32" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D32" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
           <t>2024000428</t>
         </is>
       </c>
-      <c r="B32" s="6" t="inlineStr">
+      <c r="B33" s="6" t="inlineStr">
         <is>
           <t>Miguel Moura Coelho</t>
         </is>
       </c>
-      <c r="C32" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D32" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="33"/>
-    <row r="34">
-      <c r="A34" s="2" t="inlineStr">
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D33" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="34"/>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
         <is>
           <t>TURMA: EF1801</t>
         </is>
       </c>
-      <c r="B34" s="3" t="n"/>
-      <c r="C34" s="3" t="n"/>
-      <c r="D34" s="4" t="n"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="5" t="inlineStr">
+      <c r="B35" s="3" t="n"/>
+      <c r="C35" s="3" t="n"/>
+      <c r="D35" s="4" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B35" s="5" t="inlineStr">
+      <c r="B36" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C35" s="5" t="inlineStr">
+      <c r="C36" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D35" s="5" t="inlineStr">
+      <c r="D36" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="8" t="inlineStr">
+    <row r="37">
+      <c r="A37" s="8" t="inlineStr">
         <is>
           <t>2733001117</t>
         </is>
       </c>
-      <c r="B36" s="8" t="inlineStr">
+      <c r="B37" s="8" t="inlineStr">
         <is>
           <t>Alícia José Caldararo</t>
         </is>
       </c>
-      <c r="C36" s="8" t="inlineStr">
+      <c r="C37" s="8" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D36" s="8" t="inlineStr">
+      <c r="D37" s="8" t="inlineStr">
         <is>
           <t>Entrada: 08:26:45</t>
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="7" t="inlineStr">
+    <row r="38">
+      <c r="A38" s="7" t="inlineStr">
         <is>
           <t>2006001114</t>
         </is>
       </c>
-      <c r="B37" s="7" t="inlineStr">
+      <c r="B38" s="7" t="inlineStr">
         <is>
           <t>Lucas Pena Campos Machado</t>
         </is>
       </c>
-      <c r="C37" s="7" t="inlineStr">
+      <c r="C38" s="7" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D37" s="7" t="inlineStr">
+      <c r="D38" s="7" t="inlineStr">
         <is>
           <t>Saída: 10:53:52</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="6" t="inlineStr">
-        <is>
-          <t>2024000445</t>
-        </is>
-      </c>
-      <c r="B38" s="6" t="inlineStr">
-        <is>
-          <t>Miguel Nicolato Cordeiro</t>
-        </is>
-      </c>
-      <c r="C38" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D38" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="6" t="inlineStr">
         <is>
+          <t>2024000445</t>
+        </is>
+      </c>
+      <c r="B39" s="6" t="inlineStr">
+        <is>
+          <t>Miguel Nicolato Cordeiro</t>
+        </is>
+      </c>
+      <c r="C39" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D39" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="inlineStr">
+        <is>
           <t>2011001114</t>
         </is>
       </c>
-      <c r="B39" s="6" t="inlineStr">
+      <c r="B40" s="6" t="inlineStr">
         <is>
           <t>Pedro do Almo Bustilho</t>
         </is>
       </c>
-      <c r="C39" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D39" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="40"/>
-    <row r="41">
-      <c r="A41" s="2" t="inlineStr">
+      <c r="C40" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D40" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="41"/>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
         <is>
           <t>TURMA: EF1802</t>
         </is>
       </c>
-      <c r="B41" s="3" t="n"/>
-      <c r="C41" s="3" t="n"/>
-      <c r="D41" s="4" t="n"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="5" t="inlineStr">
+      <c r="B42" s="3" t="n"/>
+      <c r="C42" s="3" t="n"/>
+      <c r="D42" s="4" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B42" s="5" t="inlineStr">
+      <c r="B43" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C42" s="5" t="inlineStr">
+      <c r="C43" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D42" s="5" t="inlineStr">
+      <c r="D43" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="6" t="inlineStr">
-        <is>
-          <t>2025000697</t>
-        </is>
-      </c>
-      <c r="B43" s="6" t="inlineStr">
-        <is>
-          <t>Maria Rosa Eccard de Souza</t>
-        </is>
-      </c>
-      <c r="C43" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D43" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="6" t="inlineStr">
         <is>
+          <t>2025000697</t>
+        </is>
+      </c>
+      <c r="B44" s="6" t="inlineStr">
+        <is>
+          <t>Maria Rosa Eccard de Souza</t>
+        </is>
+      </c>
+      <c r="C44" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D44" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
           <t>3534001122</t>
         </is>
       </c>
-      <c r="B44" s="6" t="inlineStr">
+      <c r="B45" s="6" t="inlineStr">
         <is>
           <t>Olavo Damasceno Torres</t>
         </is>
       </c>
-      <c r="C44" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D44" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="8" t="inlineStr">
+      <c r="C45" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D45" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="8" t="inlineStr">
         <is>
           <t>3256001120</t>
         </is>
       </c>
-      <c r="B45" s="8" t="inlineStr">
+      <c r="B46" s="8" t="inlineStr">
         <is>
           <t>Rayan Ribeiro Pacheco</t>
         </is>
       </c>
-      <c r="C45" s="8" t="inlineStr">
+      <c r="C46" s="8" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D45" s="8" t="inlineStr">
+      <c r="D46" s="8" t="inlineStr">
         <is>
           <t>Entrada: 08:22:34</t>
         </is>
       </c>
     </row>
-    <row r="46"/>
-    <row r="47">
-      <c r="A47" s="2" t="inlineStr">
+    <row r="47"/>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
         <is>
           <t>TURMA: EF1803</t>
         </is>
       </c>
-      <c r="B47" s="3" t="n"/>
-      <c r="C47" s="3" t="n"/>
-      <c r="D47" s="4" t="n"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="5" t="inlineStr">
+      <c r="B48" s="3" t="n"/>
+      <c r="C48" s="3" t="n"/>
+      <c r="D48" s="4" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B48" s="5" t="inlineStr">
+      <c r="B49" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C48" s="5" t="inlineStr">
+      <c r="C49" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D48" s="5" t="inlineStr">
+      <c r="D49" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="7" t="inlineStr">
-        <is>
-          <t>2023000230</t>
-        </is>
-      </c>
-      <c r="B49" s="7" t="inlineStr">
-        <is>
-          <t>Ana Alice de Souza Oliveira</t>
-        </is>
-      </c>
-      <c r="C49" s="7" t="inlineStr">
-        <is>
-          <t>SAIU CEDO</t>
-        </is>
-      </c>
-      <c r="D49" s="7" t="inlineStr">
-        <is>
-          <t>Saída: 10:56:57</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="7" t="inlineStr">
         <is>
+          <t>2023000230</t>
+        </is>
+      </c>
+      <c r="B50" s="7" t="inlineStr">
+        <is>
+          <t>Ana Alice de Souza Oliveira</t>
+        </is>
+      </c>
+      <c r="C50" s="7" t="inlineStr">
+        <is>
+          <t>SAIU CEDO</t>
+        </is>
+      </c>
+      <c r="D50" s="7" t="inlineStr">
+        <is>
+          <t>Saída: 10:56:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="7" t="inlineStr">
+        <is>
           <t>2024000497</t>
         </is>
       </c>
-      <c r="B50" s="7" t="inlineStr">
+      <c r="B51" s="7" t="inlineStr">
         <is>
           <t>Carlos Roberto Ferraz Neto</t>
         </is>
       </c>
-      <c r="C50" s="7" t="inlineStr">
+      <c r="C51" s="7" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D50" s="7" t="inlineStr">
+      <c r="D51" s="7" t="inlineStr">
         <is>
           <t>Saída: 10:10:19</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="6" t="inlineStr">
-        <is>
-          <t>2024000521</t>
-        </is>
-      </c>
-      <c r="B51" s="6" t="inlineStr">
-        <is>
-          <t>Danilo Couto Maris Guia</t>
-        </is>
-      </c>
-      <c r="C51" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D51" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="6" t="inlineStr">
         <is>
+          <t>2024000521</t>
+        </is>
+      </c>
+      <c r="B52" s="6" t="inlineStr">
+        <is>
+          <t>Danilo Couto Maris Guia</t>
+        </is>
+      </c>
+      <c r="C52" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D52" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
           <t>2022016100</t>
         </is>
       </c>
-      <c r="B52" s="6" t="inlineStr">
+      <c r="B53" s="6" t="inlineStr">
         <is>
           <t>Luisa Guimarães Boechat</t>
         </is>
       </c>
-      <c r="C52" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D52" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="53"/>
-    <row r="54">
-      <c r="A54" s="2" t="inlineStr">
+      <c r="C53" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="54"/>
+    <row r="55">
+      <c r="A55" s="2" t="inlineStr">
         <is>
           <t>TURMA: EF1901</t>
         </is>
       </c>
-      <c r="B54" s="3" t="n"/>
-      <c r="C54" s="3" t="n"/>
-      <c r="D54" s="4" t="n"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="5" t="inlineStr">
+      <c r="B55" s="3" t="n"/>
+      <c r="C55" s="3" t="n"/>
+      <c r="D55" s="4" t="n"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B55" s="5" t="inlineStr">
+      <c r="B56" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C55" s="5" t="inlineStr">
+      <c r="C56" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D55" s="5" t="inlineStr">
+      <c r="D56" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="6" t="inlineStr">
-        <is>
-          <t>3384001121</t>
-        </is>
-      </c>
-      <c r="B56" s="6" t="inlineStr">
-        <is>
-          <t>Antônio Marinho Calado</t>
-        </is>
-      </c>
-      <c r="C56" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D56" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="6" t="inlineStr">
         <is>
-          <t>2023000254</t>
+          <t>3384001121</t>
         </is>
       </c>
       <c r="B57" s="6" t="inlineStr">
         <is>
-          <t>Bernardo Thurler da Silva</t>
+          <t>Antônio Marinho Calado</t>
         </is>
       </c>
       <c r="C57" s="6" t="inlineStr">
@@ -1495,12 +1495,12 @@
     <row r="58">
       <c r="A58" s="6" t="inlineStr">
         <is>
-          <t>2194001114</t>
+          <t>2023000254</t>
         </is>
       </c>
       <c r="B58" s="6" t="inlineStr">
         <is>
-          <t>Davi de Souza Mello</t>
+          <t>Bernardo Thurler da Silva</t>
         </is>
       </c>
       <c r="C58" s="6" t="inlineStr">
@@ -1517,89 +1517,89 @@
     <row r="59">
       <c r="A59" s="6" t="inlineStr">
         <is>
+          <t>2194001114</t>
+        </is>
+      </c>
+      <c r="B59" s="6" t="inlineStr">
+        <is>
+          <t>Davi de Souza Mello</t>
+        </is>
+      </c>
+      <c r="C59" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D59" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="6" t="inlineStr">
+        <is>
           <t>2025000705</t>
         </is>
       </c>
-      <c r="B59" s="6" t="inlineStr">
+      <c r="B60" s="6" t="inlineStr">
         <is>
           <t>Sarah Emunah Alves Tavares</t>
         </is>
       </c>
-      <c r="C59" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D59" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="60"/>
-    <row r="61">
-      <c r="A61" s="2" t="inlineStr">
+      <c r="C60" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D60" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="61"/>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
         <is>
           <t>TURMA: EF1902</t>
         </is>
       </c>
-      <c r="B61" s="3" t="n"/>
-      <c r="C61" s="3" t="n"/>
-      <c r="D61" s="4" t="n"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="5" t="inlineStr">
+      <c r="B62" s="3" t="n"/>
+      <c r="C62" s="3" t="n"/>
+      <c r="D62" s="4" t="n"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B62" s="5" t="inlineStr">
+      <c r="B63" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C62" s="5" t="inlineStr">
+      <c r="C63" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D62" s="5" t="inlineStr">
+      <c r="D63" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="6" t="inlineStr">
-        <is>
-          <t>2024000455</t>
-        </is>
-      </c>
-      <c r="B63" s="6" t="inlineStr">
-        <is>
-          <t>Alícia Nicolato Cordeiro</t>
-        </is>
-      </c>
-      <c r="C63" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D63" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="6" t="inlineStr">
         <is>
-          <t>1934001113</t>
+          <t>2024000455</t>
         </is>
       </c>
       <c r="B64" s="6" t="inlineStr">
         <is>
-          <t>Gabriella Trocilo Rostagno</t>
+          <t>Alícia Nicolato Cordeiro</t>
         </is>
       </c>
       <c r="C64" s="6" t="inlineStr">
@@ -1616,78 +1616,78 @@
     <row r="65">
       <c r="A65" s="6" t="inlineStr">
         <is>
+          <t>1934001113</t>
+        </is>
+      </c>
+      <c r="B65" s="6" t="inlineStr">
+        <is>
+          <t>Gabriella Trocilo Rostagno</t>
+        </is>
+      </c>
+      <c r="C65" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D65" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="6" t="inlineStr">
+        <is>
           <t>3704001122</t>
         </is>
       </c>
-      <c r="B65" s="6" t="inlineStr">
+      <c r="B66" s="6" t="inlineStr">
         <is>
           <t>Isabela Tinoco Novaes Lannes Santucci</t>
         </is>
       </c>
-      <c r="C65" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D65" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="8" t="inlineStr">
+      <c r="C66" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D66" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="8" t="inlineStr">
         <is>
           <t>1935001113</t>
         </is>
       </c>
-      <c r="B66" s="8" t="inlineStr">
+      <c r="B67" s="8" t="inlineStr">
         <is>
           <t>Laura Zanon Branco Garibaldi</t>
         </is>
       </c>
-      <c r="C66" s="8" t="inlineStr">
+      <c r="C67" s="8" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D66" s="8" t="inlineStr">
+      <c r="D67" s="8" t="inlineStr">
         <is>
           <t>Entrada: 08:04:57</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="6" t="inlineStr">
-        <is>
-          <t>3655001122</t>
-        </is>
-      </c>
-      <c r="B67" s="6" t="inlineStr">
-        <is>
-          <t>Letícia Pinheiro Lopes</t>
-        </is>
-      </c>
-      <c r="C67" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D67" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="6" t="inlineStr">
         <is>
-          <t>2024000449</t>
+          <t>3655001122</t>
         </is>
       </c>
       <c r="B68" s="6" t="inlineStr">
         <is>
-          <t>Luiza Levate Pereira</t>
+          <t>Letícia Pinheiro Lopes</t>
         </is>
       </c>
       <c r="C68" s="6" t="inlineStr">
@@ -1704,89 +1704,89 @@
     <row r="69">
       <c r="A69" s="6" t="inlineStr">
         <is>
+          <t>2024000449</t>
+        </is>
+      </c>
+      <c r="B69" s="6" t="inlineStr">
+        <is>
+          <t>Luiza Levate Pereira</t>
+        </is>
+      </c>
+      <c r="C69" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D69" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="6" t="inlineStr">
+        <is>
           <t>2025000709</t>
         </is>
       </c>
-      <c r="B69" s="6" t="inlineStr">
+      <c r="B70" s="6" t="inlineStr">
         <is>
           <t>Maria Eduarda Faria de Souza</t>
         </is>
       </c>
-      <c r="C69" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D69" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="70"/>
-    <row r="71">
-      <c r="A71" s="2" t="inlineStr">
+      <c r="C70" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D70" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="71"/>
+    <row r="72">
+      <c r="A72" s="2" t="inlineStr">
         <is>
           <t>TURMA: EM2101</t>
         </is>
       </c>
-      <c r="B71" s="3" t="n"/>
-      <c r="C71" s="3" t="n"/>
-      <c r="D71" s="4" t="n"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="5" t="inlineStr">
+      <c r="B72" s="3" t="n"/>
+      <c r="C72" s="3" t="n"/>
+      <c r="D72" s="4" t="n"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B72" s="5" t="inlineStr">
+      <c r="B73" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C72" s="5" t="inlineStr">
+      <c r="C73" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D72" s="5" t="inlineStr">
+      <c r="D73" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="6" t="inlineStr">
-        <is>
-          <t>2025000721</t>
-        </is>
-      </c>
-      <c r="B73" s="6" t="inlineStr">
-        <is>
-          <t>Bia Bastos Sueth</t>
-        </is>
-      </c>
-      <c r="C73" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D73" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="6" t="inlineStr">
         <is>
-          <t>2025000577</t>
+          <t>2025000721</t>
         </is>
       </c>
       <c r="B74" s="6" t="inlineStr">
         <is>
-          <t>João Vitor Mangaravite Fani</t>
+          <t>Bia Bastos Sueth</t>
         </is>
       </c>
       <c r="C74" s="6" t="inlineStr">
@@ -1803,298 +1803,298 @@
     <row r="75">
       <c r="A75" s="6" t="inlineStr">
         <is>
+          <t>2025000577</t>
+        </is>
+      </c>
+      <c r="B75" s="6" t="inlineStr">
+        <is>
+          <t>João Vitor Mangaravite Fani</t>
+        </is>
+      </c>
+      <c r="C75" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D75" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="6" t="inlineStr">
+        <is>
           <t>2025000573</t>
         </is>
       </c>
-      <c r="B75" s="6" t="inlineStr">
+      <c r="B76" s="6" t="inlineStr">
         <is>
           <t>Luma de Oliveira Carvalho</t>
         </is>
       </c>
-      <c r="C75" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D75" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="8" t="inlineStr">
+      <c r="C76" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D76" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="8" t="inlineStr">
         <is>
           <t>2025000587</t>
         </is>
       </c>
-      <c r="B76" s="8" t="inlineStr">
+      <c r="B77" s="8" t="inlineStr">
         <is>
           <t>Maria Fernanda Cesar Borges</t>
         </is>
       </c>
-      <c r="C76" s="8" t="inlineStr">
+      <c r="C77" s="8" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D76" s="8" t="inlineStr">
+      <c r="D77" s="8" t="inlineStr">
         <is>
           <t>Entrada: 08:51:43</t>
         </is>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="6" t="inlineStr">
+    <row r="78">
+      <c r="A78" s="6" t="inlineStr">
         <is>
           <t>2025000579</t>
         </is>
       </c>
-      <c r="B77" s="6" t="inlineStr">
+      <c r="B78" s="6" t="inlineStr">
         <is>
           <t>Maria Luísa Gaudard Cardoso</t>
         </is>
       </c>
-      <c r="C77" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D77" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="8" t="inlineStr">
+      <c r="C78" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D78" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="8" t="inlineStr">
         <is>
           <t>2025000748</t>
         </is>
       </c>
-      <c r="B78" s="8" t="inlineStr">
+      <c r="B79" s="8" t="inlineStr">
         <is>
           <t>Matheus Coutinho Madeira</t>
         </is>
       </c>
-      <c r="C78" s="8" t="inlineStr">
+      <c r="C79" s="8" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D78" s="8" t="inlineStr">
+      <c r="D79" s="8" t="inlineStr">
         <is>
           <t>Entrada: 09:01:14</t>
         </is>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="6" t="inlineStr">
+    <row r="80">
+      <c r="A80" s="6" t="inlineStr">
         <is>
           <t>2025000608</t>
         </is>
       </c>
-      <c r="B79" s="6" t="inlineStr">
+      <c r="B80" s="6" t="inlineStr">
         <is>
           <t>Miguel Cunha Bastos Rocha</t>
         </is>
       </c>
-      <c r="C79" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D79" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="80"/>
-    <row r="81">
-      <c r="A81" s="2" t="inlineStr">
+      <c r="C80" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D80" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="81"/>
+    <row r="82">
+      <c r="A82" s="2" t="inlineStr">
         <is>
           <t>TURMA: EM2102</t>
         </is>
       </c>
-      <c r="B81" s="3" t="n"/>
-      <c r="C81" s="3" t="n"/>
-      <c r="D81" s="4" t="n"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="5" t="inlineStr">
+      <c r="B82" s="3" t="n"/>
+      <c r="C82" s="3" t="n"/>
+      <c r="D82" s="4" t="n"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B82" s="5" t="inlineStr">
+      <c r="B83" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C82" s="5" t="inlineStr">
+      <c r="C83" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D82" s="5" t="inlineStr">
+      <c r="D83" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="7" t="inlineStr">
+    <row r="84">
+      <c r="A84" s="7" t="inlineStr">
         <is>
           <t>2025000576</t>
         </is>
       </c>
-      <c r="B83" s="7" t="inlineStr">
+      <c r="B84" s="7" t="inlineStr">
         <is>
           <t>Bernardo Antonio Vieira Verdan</t>
         </is>
       </c>
-      <c r="C83" s="7" t="inlineStr">
+      <c r="C84" s="7" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D83" s="7" t="inlineStr">
+      <c r="D84" s="7" t="inlineStr">
         <is>
           <t>Saída: 11:21:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="6" t="inlineStr">
-        <is>
-          <t>2025000730</t>
-        </is>
-      </c>
-      <c r="B84" s="6" t="inlineStr">
-        <is>
-          <t>Bernardo Miccichelli Arantes Garcia</t>
-        </is>
-      </c>
-      <c r="C84" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D84" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="6" t="inlineStr">
         <is>
+          <t>2025000730</t>
+        </is>
+      </c>
+      <c r="B85" s="6" t="inlineStr">
+        <is>
+          <t>Bernardo Miccichelli Arantes Garcia</t>
+        </is>
+      </c>
+      <c r="C85" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D85" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="6" t="inlineStr">
+        <is>
           <t>2025000597</t>
         </is>
       </c>
-      <c r="B85" s="6" t="inlineStr">
+      <c r="B86" s="6" t="inlineStr">
         <is>
           <t>Maria Valentina Satolo Cucco</t>
         </is>
       </c>
-      <c r="C85" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D85" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="8" t="inlineStr">
+      <c r="C86" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D86" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="8" t="inlineStr">
         <is>
           <t>2025000610</t>
         </is>
       </c>
-      <c r="B86" s="8" t="inlineStr">
+      <c r="B87" s="8" t="inlineStr">
         <is>
           <t>Pablo da Silva Soares</t>
         </is>
       </c>
-      <c r="C86" s="8" t="inlineStr">
+      <c r="C87" s="8" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D86" s="8" t="inlineStr">
+      <c r="D87" s="8" t="inlineStr">
         <is>
           <t>Entrada: 08:35:56</t>
         </is>
       </c>
     </row>
-    <row r="87"/>
-    <row r="88">
-      <c r="A88" s="2" t="inlineStr">
+    <row r="88"/>
+    <row r="89">
+      <c r="A89" s="2" t="inlineStr">
         <is>
           <t>TURMA: EM2201</t>
         </is>
       </c>
-      <c r="B88" s="3" t="n"/>
-      <c r="C88" s="3" t="n"/>
-      <c r="D88" s="4" t="n"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="5" t="inlineStr">
+      <c r="B89" s="3" t="n"/>
+      <c r="C89" s="3" t="n"/>
+      <c r="D89" s="4" t="n"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B89" s="5" t="inlineStr">
+      <c r="B90" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C89" s="5" t="inlineStr">
+      <c r="C90" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D89" s="5" t="inlineStr">
+      <c r="D90" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="6" t="inlineStr">
-        <is>
-          <t>2024000283</t>
-        </is>
-      </c>
-      <c r="B90" s="6" t="inlineStr">
-        <is>
-          <t>Anthony Marcos Montenegro Freitas</t>
-        </is>
-      </c>
-      <c r="C90" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D90" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="6" t="inlineStr">
         <is>
-          <t>2024000311</t>
+          <t>2024000283</t>
         </is>
       </c>
       <c r="B91" s="6" t="inlineStr">
         <is>
-          <t>Arthur Boechat Pereira</t>
+          <t>Anthony Marcos Montenegro Freitas</t>
         </is>
       </c>
       <c r="C91" s="6" t="inlineStr">
@@ -2111,12 +2111,12 @@
     <row r="92">
       <c r="A92" s="6" t="inlineStr">
         <is>
-          <t>2024000301</t>
+          <t>2024000311</t>
         </is>
       </c>
       <c r="B92" s="6" t="inlineStr">
         <is>
-          <t>Arthur Rodrigues Pimentel</t>
+          <t>Arthur Boechat Pereira</t>
         </is>
       </c>
       <c r="C92" s="6" t="inlineStr">
@@ -2133,78 +2133,78 @@
     <row r="93">
       <c r="A93" s="6" t="inlineStr">
         <is>
+          <t>2024000301</t>
+        </is>
+      </c>
+      <c r="B93" s="6" t="inlineStr">
+        <is>
+          <t>Arthur Rodrigues Pimentel</t>
+        </is>
+      </c>
+      <c r="C93" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D93" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="6" t="inlineStr">
+        <is>
           <t>2024000307</t>
         </is>
       </c>
-      <c r="B93" s="6" t="inlineStr">
+      <c r="B94" s="6" t="inlineStr">
         <is>
           <t>Bernardo Moulin da Costa</t>
         </is>
       </c>
-      <c r="C93" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D93" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="7" t="inlineStr">
+      <c r="C94" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D94" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="7" t="inlineStr">
         <is>
           <t>2024000472</t>
         </is>
       </c>
-      <c r="B94" s="7" t="inlineStr">
+      <c r="B95" s="7" t="inlineStr">
         <is>
           <t>Emanuel Gonçalves Martins</t>
         </is>
       </c>
-      <c r="C94" s="7" t="inlineStr">
+      <c r="C95" s="7" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D94" s="7" t="inlineStr">
+      <c r="D95" s="7" t="inlineStr">
         <is>
           <t>Saída: 10:45:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="6" t="inlineStr">
-        <is>
-          <t>2024000278</t>
-        </is>
-      </c>
-      <c r="B95" s="6" t="inlineStr">
-        <is>
-          <t>Esther Nunes Teixeira</t>
-        </is>
-      </c>
-      <c r="C95" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D95" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="6" t="inlineStr">
         <is>
-          <t>2024000467</t>
+          <t>2024000278</t>
         </is>
       </c>
       <c r="B96" s="6" t="inlineStr">
         <is>
-          <t>Isabel Batista Moura</t>
+          <t>Esther Nunes Teixeira</t>
         </is>
       </c>
       <c r="C96" s="6" t="inlineStr">
@@ -2221,12 +2221,12 @@
     <row r="97">
       <c r="A97" s="6" t="inlineStr">
         <is>
-          <t>2024000466</t>
+          <t>2024000467</t>
         </is>
       </c>
       <c r="B97" s="6" t="inlineStr">
         <is>
-          <t>Laura Peixoto Vieira Alves</t>
+          <t>Isabel Batista Moura</t>
         </is>
       </c>
       <c r="C97" s="6" t="inlineStr">
@@ -2243,12 +2243,12 @@
     <row r="98">
       <c r="A98" s="6" t="inlineStr">
         <is>
-          <t>2025000752</t>
+          <t>2024000466</t>
         </is>
       </c>
       <c r="B98" s="6" t="inlineStr">
         <is>
-          <t>Luiza Fonseca Monteiro</t>
+          <t>Laura Peixoto Vieira Alves</t>
         </is>
       </c>
       <c r="C98" s="6" t="inlineStr">
@@ -2265,12 +2265,12 @@
     <row r="99">
       <c r="A99" s="6" t="inlineStr">
         <is>
-          <t>2024000473</t>
+          <t>2025000752</t>
         </is>
       </c>
       <c r="B99" s="6" t="inlineStr">
         <is>
-          <t>Luísa Magalhães Zanelli</t>
+          <t>Luiza Fonseca Monteiro</t>
         </is>
       </c>
       <c r="C99" s="6" t="inlineStr">
@@ -2287,12 +2287,12 @@
     <row r="100">
       <c r="A100" s="6" t="inlineStr">
         <is>
-          <t>2024000293</t>
+          <t>2024000473</t>
         </is>
       </c>
       <c r="B100" s="6" t="inlineStr">
         <is>
-          <t>Maria Vitória Figueira Torres</t>
+          <t>Luísa Magalhães Zanelli</t>
         </is>
       </c>
       <c r="C100" s="6" t="inlineStr">
@@ -2309,89 +2309,89 @@
     <row r="101">
       <c r="A101" s="6" t="inlineStr">
         <is>
+          <t>2024000293</t>
+        </is>
+      </c>
+      <c r="B101" s="6" t="inlineStr">
+        <is>
+          <t>Maria Vitória Figueira Torres</t>
+        </is>
+      </c>
+      <c r="C101" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D101" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="6" t="inlineStr">
+        <is>
           <t>2024000460</t>
         </is>
       </c>
-      <c r="B101" s="6" t="inlineStr">
+      <c r="B102" s="6" t="inlineStr">
         <is>
           <t>Welington Vioti Nascif de Mendonça Thurler</t>
         </is>
       </c>
-      <c r="C101" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D101" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="102"/>
-    <row r="103">
-      <c r="A103" s="2" t="inlineStr">
+      <c r="C102" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D102" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="103"/>
+    <row r="104">
+      <c r="A104" s="2" t="inlineStr">
         <is>
           <t>TURMA: EM2202</t>
         </is>
       </c>
-      <c r="B103" s="3" t="n"/>
-      <c r="C103" s="3" t="n"/>
-      <c r="D103" s="4" t="n"/>
-    </row>
-    <row r="104">
-      <c r="A104" s="5" t="inlineStr">
+      <c r="B104" s="3" t="n"/>
+      <c r="C104" s="3" t="n"/>
+      <c r="D104" s="4" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B104" s="5" t="inlineStr">
+      <c r="B105" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C104" s="5" t="inlineStr">
+      <c r="C105" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D104" s="5" t="inlineStr">
+      <c r="D105" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="6" t="inlineStr">
-        <is>
-          <t>2024000306</t>
-        </is>
-      </c>
-      <c r="B105" s="6" t="inlineStr">
-        <is>
-          <t>Alice Freitas de Araujo Nuss</t>
-        </is>
-      </c>
-      <c r="C105" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D105" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="6" t="inlineStr">
         <is>
-          <t>2024000313</t>
+          <t>2024000306</t>
         </is>
       </c>
       <c r="B106" s="6" t="inlineStr">
         <is>
-          <t>Beatriz Bastos Furtado</t>
+          <t>Alice Freitas de Araujo Nuss</t>
         </is>
       </c>
       <c r="C106" s="6" t="inlineStr">
@@ -2408,12 +2408,12 @@
     <row r="107">
       <c r="A107" s="6" t="inlineStr">
         <is>
-          <t>2024000275</t>
+          <t>2024000313</t>
         </is>
       </c>
       <c r="B107" s="6" t="inlineStr">
         <is>
-          <t>Daniel Coelho Schuab de Souza</t>
+          <t>Beatriz Bastos Furtado</t>
         </is>
       </c>
       <c r="C107" s="6" t="inlineStr">
@@ -2430,12 +2430,12 @@
     <row r="108">
       <c r="A108" s="6" t="inlineStr">
         <is>
-          <t>2024000300</t>
+          <t>2024000275</t>
         </is>
       </c>
       <c r="B108" s="6" t="inlineStr">
         <is>
-          <t>Gustavo Von-Held Nunes</t>
+          <t>Daniel Coelho Schuab de Souza</t>
         </is>
       </c>
       <c r="C108" s="6" t="inlineStr">
@@ -2452,12 +2452,12 @@
     <row r="109">
       <c r="A109" s="6" t="inlineStr">
         <is>
-          <t>2024000304</t>
+          <t>2024000300</t>
         </is>
       </c>
       <c r="B109" s="6" t="inlineStr">
         <is>
-          <t>João Lucas da Silva Teixeira</t>
+          <t>Gustavo Von-Held Nunes</t>
         </is>
       </c>
       <c r="C109" s="6" t="inlineStr">
@@ -2474,12 +2474,12 @@
     <row r="110">
       <c r="A110" s="6" t="inlineStr">
         <is>
-          <t>2024000458</t>
+          <t>2024000304</t>
         </is>
       </c>
       <c r="B110" s="6" t="inlineStr">
         <is>
-          <t>Letícia Alves de Souza</t>
+          <t>João Lucas da Silva Teixeira</t>
         </is>
       </c>
       <c r="C110" s="6" t="inlineStr">
@@ -2496,12 +2496,12 @@
     <row r="111">
       <c r="A111" s="6" t="inlineStr">
         <is>
-          <t>2024000470</t>
+          <t>2024000458</t>
         </is>
       </c>
       <c r="B111" s="6" t="inlineStr">
         <is>
-          <t>Lis Poeys Duarte Lopes</t>
+          <t>Letícia Alves de Souza</t>
         </is>
       </c>
       <c r="C111" s="6" t="inlineStr">
@@ -2518,12 +2518,12 @@
     <row r="112">
       <c r="A112" s="6" t="inlineStr">
         <is>
-          <t>2024000459</t>
+          <t>2024000470</t>
         </is>
       </c>
       <c r="B112" s="6" t="inlineStr">
         <is>
-          <t>Manuella Martins de Oliveira Kadour</t>
+          <t>Lis Poeys Duarte Lopes</t>
         </is>
       </c>
       <c r="C112" s="6" t="inlineStr">
@@ -2540,12 +2540,12 @@
     <row r="113">
       <c r="A113" s="6" t="inlineStr">
         <is>
-          <t>2024000277</t>
+          <t>2024000459</t>
         </is>
       </c>
       <c r="B113" s="6" t="inlineStr">
         <is>
-          <t>Maria Clara Nery Garcia</t>
+          <t>Manuella Martins de Oliveira Kadour</t>
         </is>
       </c>
       <c r="C113" s="6" t="inlineStr">
@@ -2562,12 +2562,12 @@
     <row r="114">
       <c r="A114" s="6" t="inlineStr">
         <is>
-          <t>2024000468</t>
+          <t>2024000277</t>
         </is>
       </c>
       <c r="B114" s="6" t="inlineStr">
         <is>
-          <t>Maria Luisa Silveira Nunes</t>
+          <t>Maria Clara Nery Garcia</t>
         </is>
       </c>
       <c r="C114" s="6" t="inlineStr">
@@ -2584,12 +2584,12 @@
     <row r="115">
       <c r="A115" s="6" t="inlineStr">
         <is>
-          <t>2024000475</t>
+          <t>2024000468</t>
         </is>
       </c>
       <c r="B115" s="6" t="inlineStr">
         <is>
-          <t>Miguel de Castro Costa</t>
+          <t>Maria Luisa Silveira Nunes</t>
         </is>
       </c>
       <c r="C115" s="6" t="inlineStr">
@@ -2606,12 +2606,12 @@
     <row r="116">
       <c r="A116" s="6" t="inlineStr">
         <is>
-          <t>2024000289</t>
+          <t>2024000475</t>
         </is>
       </c>
       <c r="B116" s="6" t="inlineStr">
         <is>
-          <t>Ricardo de Almeida Nunes Pessanha</t>
+          <t>Miguel de Castro Costa</t>
         </is>
       </c>
       <c r="C116" s="6" t="inlineStr">
@@ -2628,89 +2628,89 @@
     <row r="117">
       <c r="A117" s="6" t="inlineStr">
         <is>
+          <t>2024000289</t>
+        </is>
+      </c>
+      <c r="B117" s="6" t="inlineStr">
+        <is>
+          <t>Ricardo de Almeida Nunes Pessanha</t>
+        </is>
+      </c>
+      <c r="C117" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D117" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="6" t="inlineStr">
+        <is>
           <t>2024000279</t>
         </is>
       </c>
-      <c r="B117" s="6" t="inlineStr">
+      <c r="B118" s="6" t="inlineStr">
         <is>
           <t>Sophia Nuss Nogueira da Gama Costa Siqueira</t>
         </is>
       </c>
-      <c r="C117" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D117" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="118"/>
-    <row r="119">
-      <c r="A119" s="2" t="inlineStr">
+      <c r="C118" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D118" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="119"/>
+    <row r="120">
+      <c r="A120" s="2" t="inlineStr">
         <is>
           <t>TURMA: EM2301</t>
         </is>
       </c>
-      <c r="B119" s="3" t="n"/>
-      <c r="C119" s="3" t="n"/>
-      <c r="D119" s="4" t="n"/>
-    </row>
-    <row r="120">
-      <c r="A120" s="5" t="inlineStr">
+      <c r="B120" s="3" t="n"/>
+      <c r="C120" s="3" t="n"/>
+      <c r="D120" s="4" t="n"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B120" s="5" t="inlineStr">
+      <c r="B121" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C120" s="5" t="inlineStr">
+      <c r="C121" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D120" s="5" t="inlineStr">
+      <c r="D121" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="6" t="inlineStr">
-        <is>
-          <t>2023000174</t>
-        </is>
-      </c>
-      <c r="B121" s="6" t="inlineStr">
-        <is>
-          <t>Bruno de Oliveira Vieira</t>
-        </is>
-      </c>
-      <c r="C121" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D121" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="6" t="inlineStr">
         <is>
-          <t>2023000034</t>
+          <t>2023000174</t>
         </is>
       </c>
       <c r="B122" s="6" t="inlineStr">
         <is>
-          <t>Clara Cunha Bastos Rocha</t>
+          <t>Bruno de Oliveira Vieira</t>
         </is>
       </c>
       <c r="C122" s="6" t="inlineStr">
@@ -2727,78 +2727,78 @@
     <row r="123">
       <c r="A123" s="6" t="inlineStr">
         <is>
+          <t>2023000034</t>
+        </is>
+      </c>
+      <c r="B123" s="6" t="inlineStr">
+        <is>
+          <t>Clara Cunha Bastos Rocha</t>
+        </is>
+      </c>
+      <c r="C123" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D123" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="6" t="inlineStr">
+        <is>
           <t>2023000035</t>
         </is>
       </c>
-      <c r="B123" s="6" t="inlineStr">
+      <c r="B124" s="6" t="inlineStr">
         <is>
           <t>Davi Meirelles de Freitas</t>
         </is>
       </c>
-      <c r="C123" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D123" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="7" t="inlineStr">
+      <c r="C124" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D124" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="7" t="inlineStr">
         <is>
           <t>2024000256</t>
         </is>
       </c>
-      <c r="B124" s="7" t="inlineStr">
+      <c r="B125" s="7" t="inlineStr">
         <is>
           <t>Eduarda Lima Ferreira</t>
         </is>
       </c>
-      <c r="C124" s="7" t="inlineStr">
+      <c r="C125" s="7" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D124" s="7" t="inlineStr">
+      <c r="D125" s="7" t="inlineStr">
         <is>
           <t>Saída: 09:01:42</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="6" t="inlineStr">
-        <is>
-          <t>2023000155</t>
-        </is>
-      </c>
-      <c r="B125" s="6" t="inlineStr">
-        <is>
-          <t>Felipe Evaristo da Silva Marcolongo</t>
-        </is>
-      </c>
-      <c r="C125" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D125" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="6" t="inlineStr">
         <is>
-          <t>2024000487</t>
+          <t>2023000155</t>
         </is>
       </c>
       <c r="B126" s="6" t="inlineStr">
         <is>
-          <t>Gabriela Carvalho Bartolini Rodrigues da Silva</t>
+          <t>Felipe Evaristo da Silva Marcolongo</t>
         </is>
       </c>
       <c r="C126" s="6" t="inlineStr">
@@ -2815,12 +2815,12 @@
     <row r="127">
       <c r="A127" s="6" t="inlineStr">
         <is>
-          <t>2023000041</t>
+          <t>2024000487</t>
         </is>
       </c>
       <c r="B127" s="6" t="inlineStr">
         <is>
-          <t>Giovanna Lopes Medina</t>
+          <t>Gabriela Carvalho Bartolini Rodrigues da Silva</t>
         </is>
       </c>
       <c r="C127" s="6" t="inlineStr">
@@ -2837,12 +2837,12 @@
     <row r="128">
       <c r="A128" s="6" t="inlineStr">
         <is>
-          <t>2023000052</t>
+          <t>2023000041</t>
         </is>
       </c>
       <c r="B128" s="6" t="inlineStr">
         <is>
-          <t>João Pedro Mançano Bastos da Cruz</t>
+          <t>Giovanna Lopes Medina</t>
         </is>
       </c>
       <c r="C128" s="6" t="inlineStr">
@@ -2859,12 +2859,12 @@
     <row r="129">
       <c r="A129" s="6" t="inlineStr">
         <is>
-          <t>2023000057</t>
+          <t>2023000052</t>
         </is>
       </c>
       <c r="B129" s="6" t="inlineStr">
         <is>
-          <t>Letícia Valeriote de Oliveira Coelho</t>
+          <t>João Pedro Mançano Bastos da Cruz</t>
         </is>
       </c>
       <c r="C129" s="6" t="inlineStr">
@@ -2881,12 +2881,12 @@
     <row r="130">
       <c r="A130" s="6" t="inlineStr">
         <is>
-          <t>2023000060</t>
+          <t>2023000057</t>
         </is>
       </c>
       <c r="B130" s="6" t="inlineStr">
         <is>
-          <t>Luíza Arantes Rangel Muniz</t>
+          <t>Letícia Valeriote de Oliveira Coelho</t>
         </is>
       </c>
       <c r="C130" s="6" t="inlineStr">
@@ -2903,12 +2903,12 @@
     <row r="131">
       <c r="A131" s="6" t="inlineStr">
         <is>
-          <t>2023000061</t>
+          <t>2023000060</t>
         </is>
       </c>
       <c r="B131" s="6" t="inlineStr">
         <is>
-          <t>Marcelly Lima de Jesus</t>
+          <t>Luíza Arantes Rangel Muniz</t>
         </is>
       </c>
       <c r="C131" s="6" t="inlineStr">
@@ -2925,12 +2925,12 @@
     <row r="132">
       <c r="A132" s="6" t="inlineStr">
         <is>
-          <t>2023000066</t>
+          <t>2023000061</t>
         </is>
       </c>
       <c r="B132" s="6" t="inlineStr">
         <is>
-          <t>Mariana Dias Carnevale</t>
+          <t>Marcelly Lima de Jesus</t>
         </is>
       </c>
       <c r="C132" s="6" t="inlineStr">
@@ -2947,12 +2947,12 @@
     <row r="133">
       <c r="A133" s="6" t="inlineStr">
         <is>
-          <t>2024000504</t>
+          <t>2023000066</t>
         </is>
       </c>
       <c r="B133" s="6" t="inlineStr">
         <is>
-          <t>Murilo Kunze Soares</t>
+          <t>Mariana Dias Carnevale</t>
         </is>
       </c>
       <c r="C133" s="6" t="inlineStr">
@@ -2969,12 +2969,12 @@
     <row r="134">
       <c r="A134" s="6" t="inlineStr">
         <is>
-          <t>2023000202</t>
+          <t>2024000504</t>
         </is>
       </c>
       <c r="B134" s="6" t="inlineStr">
         <is>
-          <t>Patrícia Resende Rodrigues da Silva</t>
+          <t>Murilo Kunze Soares</t>
         </is>
       </c>
       <c r="C134" s="6" t="inlineStr">
@@ -2991,89 +2991,89 @@
     <row r="135">
       <c r="A135" s="6" t="inlineStr">
         <is>
+          <t>2023000202</t>
+        </is>
+      </c>
+      <c r="B135" s="6" t="inlineStr">
+        <is>
+          <t>Patrícia Resende Rodrigues da Silva</t>
+        </is>
+      </c>
+      <c r="C135" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D135" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="6" t="inlineStr">
+        <is>
           <t>2023000178</t>
         </is>
       </c>
-      <c r="B135" s="6" t="inlineStr">
+      <c r="B136" s="6" t="inlineStr">
         <is>
           <t>Talles Campos Carneiro Periard</t>
         </is>
       </c>
-      <c r="C135" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D135" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="136"/>
-    <row r="137">
-      <c r="A137" s="2" t="inlineStr">
+      <c r="C136" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D136" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="137"/>
+    <row r="138">
+      <c r="A138" s="2" t="inlineStr">
         <is>
           <t>TURMA: EM2302</t>
         </is>
       </c>
-      <c r="B137" s="3" t="n"/>
-      <c r="C137" s="3" t="n"/>
-      <c r="D137" s="4" t="n"/>
-    </row>
-    <row r="138">
-      <c r="A138" s="5" t="inlineStr">
+      <c r="B138" s="3" t="n"/>
+      <c r="C138" s="3" t="n"/>
+      <c r="D138" s="4" t="n"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="5" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B138" s="5" t="inlineStr">
+      <c r="B139" s="5" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C138" s="5" t="inlineStr">
+      <c r="C139" s="5" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D138" s="5" t="inlineStr">
+      <c r="D139" s="5" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="6" t="inlineStr">
-        <is>
-          <t>2023000028</t>
-        </is>
-      </c>
-      <c r="B139" s="6" t="inlineStr">
-        <is>
-          <t>Alice Pereira Baptista</t>
-        </is>
-      </c>
-      <c r="C139" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D139" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="6" t="inlineStr">
         <is>
-          <t>2023000029</t>
+          <t>2023000028</t>
         </is>
       </c>
       <c r="B140" s="6" t="inlineStr">
         <is>
-          <t>Alice Poubel Vieira</t>
+          <t>Alice Pereira Baptista</t>
         </is>
       </c>
       <c r="C140" s="6" t="inlineStr">
@@ -3090,12 +3090,12 @@
     <row r="141">
       <c r="A141" s="6" t="inlineStr">
         <is>
-          <t>2023000168</t>
+          <t>2023000029</t>
         </is>
       </c>
       <c r="B141" s="6" t="inlineStr">
         <is>
-          <t>Ana Luísa Petterman Galito</t>
+          <t>Alice Poubel Vieira</t>
         </is>
       </c>
       <c r="C141" s="6" t="inlineStr">
@@ -3112,12 +3112,12 @@
     <row r="142">
       <c r="A142" s="6" t="inlineStr">
         <is>
-          <t>2024000484</t>
+          <t>2023000168</t>
         </is>
       </c>
       <c r="B142" s="6" t="inlineStr">
         <is>
-          <t>Ana Luísa Poubel de Souza Sampaio</t>
+          <t>Ana Luísa Petterman Galito</t>
         </is>
       </c>
       <c r="C142" s="6" t="inlineStr">
@@ -3134,12 +3134,12 @@
     <row r="143">
       <c r="A143" s="6" t="inlineStr">
         <is>
-          <t>2024000485</t>
+          <t>2024000484</t>
         </is>
       </c>
       <c r="B143" s="6" t="inlineStr">
         <is>
-          <t>Anabella Moreira de Oliveira</t>
+          <t>Ana Luísa Poubel de Souza Sampaio</t>
         </is>
       </c>
       <c r="C143" s="6" t="inlineStr">
@@ -3156,12 +3156,12 @@
     <row r="144">
       <c r="A144" s="6" t="inlineStr">
         <is>
-          <t>2023000218</t>
+          <t>2024000485</t>
         </is>
       </c>
       <c r="B144" s="6" t="inlineStr">
         <is>
-          <t>Arthur Ponciano Frontelmo Rangel</t>
+          <t>Anabella Moreira de Oliveira</t>
         </is>
       </c>
       <c r="C144" s="6" t="inlineStr">
@@ -3178,12 +3178,12 @@
     <row r="145">
       <c r="A145" s="6" t="inlineStr">
         <is>
-          <t>2023000033</t>
+          <t>2023000218</t>
         </is>
       </c>
       <c r="B145" s="6" t="inlineStr">
         <is>
-          <t>Carolina Rodrigues de Britto</t>
+          <t>Arthur Ponciano Frontelmo Rangel</t>
         </is>
       </c>
       <c r="C145" s="6" t="inlineStr">
@@ -3200,12 +3200,12 @@
     <row r="146">
       <c r="A146" s="6" t="inlineStr">
         <is>
-          <t>2023000039</t>
+          <t>2023000033</t>
         </is>
       </c>
       <c r="B146" s="6" t="inlineStr">
         <is>
-          <t>Diana Alves Fortuna Pussiareli</t>
+          <t>Carolina Rodrigues de Britto</t>
         </is>
       </c>
       <c r="C146" s="6" t="inlineStr">
@@ -3222,12 +3222,12 @@
     <row r="147">
       <c r="A147" s="6" t="inlineStr">
         <is>
-          <t>2023000145</t>
+          <t>2023000039</t>
         </is>
       </c>
       <c r="B147" s="6" t="inlineStr">
         <is>
-          <t>Décio Macedo Netto</t>
+          <t>Diana Alves Fortuna Pussiareli</t>
         </is>
       </c>
       <c r="C147" s="6" t="inlineStr">
@@ -3244,12 +3244,12 @@
     <row r="148">
       <c r="A148" s="6" t="inlineStr">
         <is>
-          <t>2025000742</t>
+          <t>2023000145</t>
         </is>
       </c>
       <c r="B148" s="6" t="inlineStr">
         <is>
-          <t>Gabriel Guilherme Ribeiro</t>
+          <t>Décio Macedo Netto</t>
         </is>
       </c>
       <c r="C148" s="6" t="inlineStr">
@@ -3266,12 +3266,12 @@
     <row r="149">
       <c r="A149" s="6" t="inlineStr">
         <is>
-          <t>2023000042</t>
+          <t>2025000742</t>
         </is>
       </c>
       <c r="B149" s="6" t="inlineStr">
         <is>
-          <t>Giovana Souza Ângelo Leite</t>
+          <t>Gabriel Guilherme Ribeiro</t>
         </is>
       </c>
       <c r="C149" s="6" t="inlineStr">
@@ -3288,12 +3288,12 @@
     <row r="150">
       <c r="A150" s="6" t="inlineStr">
         <is>
-          <t>2023000046</t>
+          <t>2023000042</t>
         </is>
       </c>
       <c r="B150" s="6" t="inlineStr">
         <is>
-          <t>Guilherme de Oliveira Avelino</t>
+          <t>Giovana Souza Ângelo Leite</t>
         </is>
       </c>
       <c r="C150" s="6" t="inlineStr">
@@ -3310,12 +3310,12 @@
     <row r="151">
       <c r="A151" s="6" t="inlineStr">
         <is>
-          <t>2023000043</t>
+          <t>2023000046</t>
         </is>
       </c>
       <c r="B151" s="6" t="inlineStr">
         <is>
-          <t>Gustavo Martins Moura Cruz</t>
+          <t>Guilherme de Oliveira Avelino</t>
         </is>
       </c>
       <c r="C151" s="6" t="inlineStr">
@@ -3332,78 +3332,78 @@
     <row r="152">
       <c r="A152" s="6" t="inlineStr">
         <is>
+          <t>2023000043</t>
+        </is>
+      </c>
+      <c r="B152" s="6" t="inlineStr">
+        <is>
+          <t>Gustavo Martins Moura Cruz</t>
+        </is>
+      </c>
+      <c r="C152" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D152" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="6" t="inlineStr">
+        <is>
           <t>2023000049</t>
         </is>
       </c>
-      <c r="B152" s="6" t="inlineStr">
+      <c r="B153" s="6" t="inlineStr">
         <is>
           <t>Isabela Poeys Rocha</t>
         </is>
       </c>
-      <c r="C152" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D152" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="8" t="inlineStr">
+      <c r="C153" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D153" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="8" t="inlineStr">
         <is>
           <t>2023000050</t>
         </is>
       </c>
-      <c r="B153" s="8" t="inlineStr">
+      <c r="B154" s="8" t="inlineStr">
         <is>
           <t>João Lucas Ximenes Diniz</t>
         </is>
       </c>
-      <c r="C153" s="8" t="inlineStr">
+      <c r="C154" s="8" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D153" s="8" t="inlineStr">
+      <c r="D154" s="8" t="inlineStr">
         <is>
           <t>Entrada: 10:41:17</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" s="6" t="inlineStr">
-        <is>
-          <t>2023000223</t>
-        </is>
-      </c>
-      <c r="B154" s="6" t="inlineStr">
-        <is>
-          <t>Julia Olmo Cabral Martins</t>
-        </is>
-      </c>
-      <c r="C154" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D154" s="6" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="6" t="inlineStr">
         <is>
-          <t>2023000054</t>
+          <t>2023000223</t>
         </is>
       </c>
       <c r="B155" s="6" t="inlineStr">
         <is>
-          <t>Júlia Montovani Patrício</t>
+          <t>Julia Olmo Cabral Martins</t>
         </is>
       </c>
       <c r="C155" s="6" t="inlineStr">
@@ -3420,12 +3420,12 @@
     <row r="156">
       <c r="A156" s="6" t="inlineStr">
         <is>
-          <t>2023000166</t>
+          <t>2023000054</t>
         </is>
       </c>
       <c r="B156" s="6" t="inlineStr">
         <is>
-          <t>Lícia Tinoco Dias</t>
+          <t>Júlia Montovani Patrício</t>
         </is>
       </c>
       <c r="C156" s="6" t="inlineStr">
@@ -3442,12 +3442,12 @@
     <row r="157">
       <c r="A157" s="6" t="inlineStr">
         <is>
-          <t>2023000160</t>
+          <t>2023000166</t>
         </is>
       </c>
       <c r="B157" s="6" t="inlineStr">
         <is>
-          <t>Manuela da Silveira Lestayo</t>
+          <t>Lícia Tinoco Dias</t>
         </is>
       </c>
       <c r="C157" s="6" t="inlineStr">
@@ -3464,12 +3464,12 @@
     <row r="158">
       <c r="A158" s="6" t="inlineStr">
         <is>
-          <t>2023000063</t>
+          <t>2023000160</t>
         </is>
       </c>
       <c r="B158" s="6" t="inlineStr">
         <is>
-          <t>Maria Júlia Faria de Souza Botelho</t>
+          <t>Manuela da Silveira Lestayo</t>
         </is>
       </c>
       <c r="C158" s="6" t="inlineStr">
@@ -3486,12 +3486,12 @@
     <row r="159">
       <c r="A159" s="6" t="inlineStr">
         <is>
-          <t>2023000227</t>
+          <t>2023000063</t>
         </is>
       </c>
       <c r="B159" s="6" t="inlineStr">
         <is>
-          <t>Maria Luísa Salles Figueiredo</t>
+          <t>Maria Júlia Faria de Souza Botelho</t>
         </is>
       </c>
       <c r="C159" s="6" t="inlineStr">
@@ -3508,12 +3508,12 @@
     <row r="160">
       <c r="A160" s="6" t="inlineStr">
         <is>
-          <t>2024000482</t>
+          <t>2023000227</t>
         </is>
       </c>
       <c r="B160" s="6" t="inlineStr">
         <is>
-          <t>Natália Costa de Castro</t>
+          <t>Maria Luísa Salles Figueiredo</t>
         </is>
       </c>
       <c r="C160" s="6" t="inlineStr">
@@ -3530,12 +3530,12 @@
     <row r="161">
       <c r="A161" s="6" t="inlineStr">
         <is>
-          <t>2023000006</t>
+          <t>2024000482</t>
         </is>
       </c>
       <c r="B161" s="6" t="inlineStr">
         <is>
-          <t>Pedro da Silva Pereira Ferreira</t>
+          <t>Natália Costa de Castro</t>
         </is>
       </c>
       <c r="C161" s="6" t="inlineStr">
@@ -3552,12 +3552,12 @@
     <row r="162">
       <c r="A162" s="6" t="inlineStr">
         <is>
-          <t>2023000074</t>
+          <t>2023000006</t>
         </is>
       </c>
       <c r="B162" s="6" t="inlineStr">
         <is>
-          <t>Rafael Tinoco Novaes Lannes Santucci</t>
+          <t>Pedro da Silva Pereira Ferreira</t>
         </is>
       </c>
       <c r="C162" s="6" t="inlineStr">
@@ -3574,12 +3574,12 @@
     <row r="163">
       <c r="A163" s="6" t="inlineStr">
         <is>
-          <t>2023000076</t>
+          <t>2023000074</t>
         </is>
       </c>
       <c r="B163" s="6" t="inlineStr">
         <is>
-          <t>Ray da Silva Martins Bizarro</t>
+          <t>Rafael Tinoco Novaes Lannes Santucci</t>
         </is>
       </c>
       <c r="C163" s="6" t="inlineStr">
@@ -3596,12 +3596,12 @@
     <row r="164">
       <c r="A164" s="6" t="inlineStr">
         <is>
-          <t>2025000758</t>
+          <t>2023000076</t>
         </is>
       </c>
       <c r="B164" s="6" t="inlineStr">
         <is>
-          <t>Víctor Machado Perusso de Souza</t>
+          <t>Ray da Silva Martins Bizarro</t>
         </is>
       </c>
       <c r="C164" s="6" t="inlineStr">
@@ -3618,20 +3618,42 @@
     <row r="165">
       <c r="A165" s="6" t="inlineStr">
         <is>
+          <t>2025000758</t>
+        </is>
+      </c>
+      <c r="B165" s="6" t="inlineStr">
+        <is>
+          <t>Víctor Machado Perusso de Souza</t>
+        </is>
+      </c>
+      <c r="C165" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D165" s="6" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="6" t="inlineStr">
+        <is>
           <t>2023000027</t>
         </is>
       </c>
-      <c r="B165" s="6" t="inlineStr">
+      <c r="B166" s="6" t="inlineStr">
         <is>
           <t>Ágata Priscila André Tarouquela</t>
         </is>
       </c>
-      <c r="C165" s="6" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D165" s="6" t="inlineStr">
+      <c r="C166" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D166" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
@@ -3640,21 +3662,21 @@
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A88:D88"/>
-    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A20:D20"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A104:D104"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A138:D138"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>